<commit_message>
update shop picture and url
</commit_message>
<xml_diff>
--- a/Web Crawler/Start research.xlsx
+++ b/Web Crawler/Start research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SAD\Web Crawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447346AD-1C0A-490F-A06A-F7D4DF141B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43DF894-9E2E-46C7-9500-64C6CE25031D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start research" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="543">
   <si>
     <t>Store Name</t>
   </si>
@@ -692,12 +692,6 @@
     <t>https://www.google.com/maps/place/%E6%8B%89%E9%BA%B5%E3%82%89%E3%81%81%E9%BA%BA%E9%AD%9A%E5%A0%BA-%E5%A4%A7%E5%AE%89%E5%BA%97/@25.0237823,121.5202943,14.26z/data=!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442ab77a4b0b4ad:0x661e0e6e46a0be8f!8m2!3d25.0266536!4d121.5394228!15sCgbmi4npurVaCCIG5ouJ6bq1kgEQcmFtZW5fcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11vyhbtv_k?entry=ttu&amp;g_ep=EgoyMDI1MDUxNS4xIKXMDSoASAFQAw%3D%3D</t>
   </si>
   <si>
-    <t>啦啦麵 24h無人拉麵店-台大店</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/%E5%95%A6%E5%95%A6%E9%BA%B5+24h%E7%84%A1%E4%BA%BA%E6%8B%89%E9%BA%B5%E5%BA%97-%E5%8F%B0%E5%A4%A7%E5%BA%97/@25.0128537,121.5057596,14z/data=!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442a93f837fec61:0x89020ea696473ca9!8m2!3d25.0128537!4d121.5359155!15sCgbmi4npurVaCCIG5ouJ6bq1kgEQcmFtZW5fcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11vwnz6k0w?entry=ttu&amp;g_ep=EgoyMDI1MDUxNS4xIKXMDSoASAFQAw%3D%3D</t>
-  </si>
-  <si>
     <t>山嵐拉麵 大安店</t>
   </si>
   <si>
@@ -725,9 +719,6 @@
     <t>https://www.google.com/maps/place/%E8%B5%A4%E6%8B%89%E9%BA%B5+Red+Ramen+%E9%B7%84%E7%99%BD%E6%B9%AF%E6%8B%89%E9%BA%B5/@25.0128537,121.5057596,14z/data=!3m1!5s0x3442aa33e22255fd:0xdef3be19876d11e!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442ab2a4fabbd3b:0x2ce0dcd450823288!8m2!3d25.0240309!4d121.5530763!15sCgbmi4npurVaCCIG5ouJ6bq1kgEQcmFtZW5fcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11mcq23gfh?entry=ttu&amp;g_ep=EgoyMDI1MDUxNS4xIKXMDSoASAFQAw%3D%3D</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/%E5%A5%BD%E5%91%B7%E6%8B%89%E9%BA%B5+%E7%94%9C%E5%93%81%E5%90%83%E5%88%B0%E9%A3%BD(%E5%B8%AB%E5%A4%A7)/@25.0128537,121.5057596,14z/data=!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442a9edc87fd46d:0x96bddbc35922fb3a!8m2!3d25.0241628!4d121.5292501!15sCgbmi4npurVaCCIG5ouJ6bq1kgEQcmFtZW5fcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11xclkz21j?entry=ttu&amp;g_ep=EgoyMDI1MDUxNS4xIKXMDSoASAFQAw%3D%3D</t>
-  </si>
-  <si>
     <t>好呷拉麵 甜品吃到飽(師大)</t>
   </si>
   <si>
@@ -824,12 +815,6 @@
     <t>https://www.google.com/maps/place/%E4%BC%8A%E7%A6%BE%E7%99%BD%E6%B9%AF/@25.0414974,121.4674319,13z/data=!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442ab68691ab6d3:0xf32b841d25339852!8m2!3d25.0319551!4d121.558028!15sCgbmi4npurVaCCIG5ouJ6bq1kgEQcmFtZW5fcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11syktvgb5?entry=ttu&amp;g_ep=EgoyMDI1MDUxNS4xIKXMDSoASAFQAw%3D%3D</t>
   </si>
   <si>
-    <t>安娜拉 24小時無人拉麵店（Annalamoon 24hours Ramen Restaurant）</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/%E5%AE%89%E5%A8%9C%E6%8B%89+24%E5%B0%8F%E6%99%82%E7%84%A1%E4%BA%BA%E6%8B%89%E9%BA%B5%E5%BA%97%EF%BC%88Annalamoon+24hours+Ramen+Restaurant%EF%BC%89/@25.0350542,121.485257,14.32z/data=!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442a9550cbae6d5:0xe711dd0f3182a578!8m2!3d25.043007!4d121.5045!15sCgbmi4npurVaCCIG5ouJ6bq1kgEKcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11w1xn8g3_?entry=ttu&amp;g_ep=EgoyMDI1MDUxNS4xIKXMDSoASAFQAw%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.google.com/maps/place/%E6%98%8E+%E6%8B%89%E9%BA%B5%E5%90%A7+MING+Ramen+Bar/@25.0350542,121.485257,14.32z/data=!3m1!5s0x3442a96dbd7b615f:0xfbdf3f86c4db5661!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442a90ae5d3d693:0x6c862e95ee922798!8m2!3d25.0496611!4d121.5169979!15sCgbmi4npurVaCCIG5ouJ6bq1kgEQcmFtZW5fcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11lv_yfvhf?entry=ttu&amp;g_ep=EgoyMDI1MDUxNS4xIKXMDSoASAFQAw%3D%3D</t>
   </si>
   <si>
@@ -927,24 +912,12 @@
   </si>
   <si>
     <t>丸吉左衛門東京醬油豚骨拉麵</t>
-  </si>
-  <si>
-    <t>韓金湯匙 無人拉麵 24 Hours (輔大店）</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/%E9%9F%93%E9%87%91%E6%B9%AF%E5%8C%99+%E7%84%A1%E4%BA%BA%E6%8B%89%E9%BA%B5+24+Hours+(%E8%BC%94%E5%A4%A7%E5%BA%97%EF%BC%89/@25.0335224,121.3961335,14z/data=!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442a764a7f83f47:0xba9dbc46d66721c1!8m2!3d25.0313812!4d121.4337388!15sCgbmi4npurVaCCIG5ouJ6bq1kgEKcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11y30_9sh2?entry=ttu&amp;g_ep=EgoyMDI1MDUxNS4xIKXMDSoASAFQAw%3D%3D</t>
   </si>
   <si>
     <t>https://www.google.com/maps/place/%E4%B8%B8%E5%90%89%E5%B7%A6%E8%A1%9B%E9%96%80%E6%9D%B1%E4%BA%AC%E9%86%AC%E6%B2%B9%E8%B1%9A%E9%AA%A8%E6%8B%89%E9%BA%B5/@25.0335224,121.3961335,14z/data=!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442a78b54bb7a17:0xbe83da081c614bc4!8m2!3d25.0226631!4d121.4229622!15sCgbmi4npurVaCCIG5ouJ6bq1kgEQcmFtZW5fcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11f55kbn8k?entry=ttu&amp;g_ep=EgoyMDI1MDUxNS4xIKXMDSoASAFQAw%3D%3D</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>吃碗拉麵再走</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/%E5%90%83%E7%A2%97%E6%8B%89%E9%BA%B5%E5%86%8D%E8%B5%B0/@25.0335224,121.3961335,14z/data=!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442a7544f52ecbf:0xc6552b193ddd5def!8m2!3d25.0307848!4d121.434075!15sCgbmi4npurVaCCIG5ouJ6bq1kgEKcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11y46_rzht?entry=ttu&amp;g_ep=EgoyMDI1MDUxNS4xIKXMDSoASAFQAw%3D%3D</t>
-  </si>
-  <si>
     <t>麵匡匡拉麵食堂 新莊富國店</t>
   </si>
   <si>
@@ -1674,6 +1647,16 @@
   </si>
   <si>
     <t>https://www.google.com/maps/place/%E9%BA%B5%E5%B1%8B%E5%8D%81%E5%85%AB%E7%94%B2/@25.0559037,121.3961567,14z/data=!4m11!1m3!2m2!1z5pel5byP5ouJ6bq1!6e5!3m6!1s0x3442a791e0321cab:0x3fc7dbc45f36fd47!8m2!3d25.0559037!4d121.4322056!15sCgzml6XlvI_mi4npurVaECIO5pelIOW8jyDmi4npurWSARByYW1lbl9yZXN0YXVyYW50qgFVCggvbS8wOWdtcxABKhIiDuaXpSDlvI8g5ouJ6bq1KEUyHxABIhtseEn-IoNAw85italN9nc7rkrvp_prWDK8ioQyEhACIg7ml6Ug5byPIOaLiem6teABAA!16s%2Fg%2F11fkt59w_j?entry=ttu&amp;g_ep=EgoyMDI1MDUyMS4wIKXMDSoASAFQAw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/%E5%A5%BD%E5%91%B7%E6%8B%89%E9%BA%B5+%E7%94%9C%E5%93%81%E5%90%83%E5%88%B0%E9%A3%BD(%E5%B8%AB%E5%A4%A7)/@25.0128537,121.5057596,14z/data=!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442a9edc87fd46d:0x96bddbc35922fb3a!8m2!3d25.0241628!4d121.5292501!15sCgbmi4npurVaCCIG5ouJ6bq1kgEQcmFtZW5fcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11xclkz21j?entry=ttu&amp;g_ep=EgoyMDI1MDUxNS4xIKXMDSoASAFQAw%3D%3D</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>李好拉麵</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/%E6%9D%8E%E5%A5%BD%E6%8B%89%E9%BA%B5/@25.0498145,121.5146039,15.68z/data=!4m11!1m3!2m2!1z5ouJ6bq1!6e5!3m6!1s0x3442abcd172a24f9:0x651dbe483a714637!8m2!3d25.0513733!4d121.5294634!15sCgbmi4npurVaCCIG5ouJ6bq1kgEQcmFtZW5fcmVzdGF1cmFudKoBRAoIL20vMDlnbXMQASoKIgbmi4npurUoRTIeEAEiGiiKbHPmyKMJ2SM2J4NGBmfVZtAASWiPucwDMgoQAiIG5ouJ6bq14AEA!16s%2Fg%2F11h4g914lf?entry=ttu&amp;g_ep=EgoyMDI1MDUyMS4wIKXMDSoASAFQAw%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -3143,10 +3126,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13038546-05B0-4609-87E5-AAC72F1A7155}">
-  <dimension ref="A1:B154"/>
+  <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView zoomScale="122" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="122" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -3165,50 +3148,50 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="B3" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="B5" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="B6" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B7" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3216,23 +3199,23 @@
         <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="B9" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B10" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3245,106 +3228,106 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B12" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B13" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="B14" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="B15" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="B16" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="B17" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="B18" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="B19" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="B20" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="B21" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="B22" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B23" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="B24" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -3357,162 +3340,162 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="B27" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B29" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="B30" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B31" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="B32" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B33" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B34" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B35" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="B36" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="B37" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="B38" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B39" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="B40" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="B41" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B42" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B43" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B44" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="B45" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -3520,876 +3503,844 @@
         <v>112</v>
       </c>
       <c r="B46" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="B47" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>304</v>
+        <v>253</v>
       </c>
       <c r="B48" t="s">
-        <v>305</v>
+        <v>254</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>256</v>
-      </c>
-      <c r="B49" t="s">
-        <v>257</v>
+        <v>231</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>234</v>
+        <v>470</v>
       </c>
       <c r="B50" t="s">
-        <v>233</v>
+        <v>471</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>266</v>
+        <v>440</v>
       </c>
       <c r="B51" t="s">
-        <v>267</v>
+        <v>441</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>479</v>
+        <v>378</v>
       </c>
       <c r="B52" t="s">
-        <v>480</v>
+        <v>379</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>449</v>
+        <v>418</v>
       </c>
       <c r="B53" t="s">
-        <v>450</v>
+        <v>419</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>387</v>
+        <v>450</v>
       </c>
       <c r="B54" t="s">
-        <v>388</v>
+        <v>451</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>427</v>
+        <v>442</v>
       </c>
       <c r="B55" t="s">
-        <v>428</v>
+        <v>443</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>459</v>
+        <v>430</v>
       </c>
       <c r="B56" t="s">
-        <v>460</v>
+        <v>431</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>451</v>
+        <v>229</v>
       </c>
       <c r="B57" t="s">
-        <v>452</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>439</v>
+        <v>386</v>
       </c>
       <c r="B58" t="s">
-        <v>440</v>
+        <v>387</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>231</v>
+        <v>291</v>
       </c>
       <c r="B59" t="s">
-        <v>232</v>
+        <v>292</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>395</v>
+        <v>458</v>
       </c>
       <c r="B60" t="s">
-        <v>396</v>
+        <v>459</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>296</v>
+        <v>490</v>
       </c>
       <c r="B61" t="s">
-        <v>297</v>
+        <v>491</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>467</v>
+        <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>468</v>
+        <v>268</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>499</v>
+        <v>335</v>
       </c>
       <c r="B63" t="s">
-        <v>500</v>
+        <v>336</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>283</v>
       </c>
       <c r="B64" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>344</v>
+        <v>462</v>
       </c>
       <c r="B65" t="s">
-        <v>345</v>
+        <v>463</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>288</v>
+        <v>220</v>
       </c>
       <c r="B66" t="s">
-        <v>289</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>471</v>
+        <v>195</v>
       </c>
       <c r="B67" t="s">
-        <v>472</v>
+        <v>263</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>220</v>
+        <v>474</v>
       </c>
       <c r="B68" t="s">
-        <v>221</v>
+        <v>475</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>195</v>
+        <v>384</v>
       </c>
       <c r="B69" t="s">
-        <v>268</v>
+        <v>385</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>483</v>
-      </c>
-      <c r="B70" t="s">
-        <v>484</v>
+        <v>323</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>393</v>
+        <v>239</v>
       </c>
       <c r="B71" t="s">
-        <v>394</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>332</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>333</v>
+        <v>416</v>
+      </c>
+      <c r="B72" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>242</v>
+        <v>341</v>
       </c>
       <c r="B73" t="s">
-        <v>243</v>
+        <v>342</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>425</v>
+        <v>233</v>
       </c>
       <c r="B74" t="s">
-        <v>426</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>350</v>
+        <v>321</v>
       </c>
       <c r="B75" t="s">
-        <v>351</v>
+        <v>322</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>236</v>
+        <v>271</v>
       </c>
       <c r="B76" t="s">
-        <v>235</v>
+        <v>272</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>330</v>
+        <v>307</v>
       </c>
       <c r="B77" t="s">
-        <v>331</v>
+        <v>308</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="B78" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>316</v>
+        <v>468</v>
       </c>
       <c r="B79" t="s">
-        <v>317</v>
+        <v>469</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>269</v>
+        <v>327</v>
       </c>
       <c r="B80" t="s">
-        <v>270</v>
+        <v>328</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>477</v>
+        <v>319</v>
       </c>
       <c r="B81" t="s">
-        <v>478</v>
+        <v>320</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>336</v>
+        <v>100</v>
       </c>
       <c r="B82" t="s">
-        <v>337</v>
+        <v>228</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>328</v>
+        <v>370</v>
       </c>
       <c r="B83" t="s">
-        <v>329</v>
+        <v>371</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>100</v>
+        <v>372</v>
       </c>
       <c r="B84" t="s">
-        <v>230</v>
+        <v>373</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>379</v>
+        <v>299</v>
       </c>
       <c r="B85" t="s">
-        <v>380</v>
+        <v>300</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B86" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>222</v>
+        <v>380</v>
       </c>
       <c r="B87" t="s">
-        <v>223</v>
+        <v>381</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>308</v>
+        <v>362</v>
       </c>
       <c r="B88" t="s">
-        <v>309</v>
+        <v>363</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>385</v>
+        <v>406</v>
       </c>
       <c r="B89" t="s">
-        <v>386</v>
+        <v>407</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>389</v>
+        <v>424</v>
       </c>
       <c r="B90" t="s">
-        <v>390</v>
+        <v>425</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>371</v>
+        <v>484</v>
       </c>
       <c r="B91" t="s">
-        <v>372</v>
+        <v>485</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>415</v>
+        <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>416</v>
+        <v>217</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>433</v>
+        <v>466</v>
       </c>
       <c r="B93" t="s">
-        <v>434</v>
+        <v>467</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>493</v>
+        <v>354</v>
       </c>
       <c r="B94" t="s">
-        <v>494</v>
+        <v>355</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>360</v>
       </c>
       <c r="B95" t="s">
-        <v>217</v>
+        <v>361</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>475</v>
+        <v>52</v>
       </c>
       <c r="B96" t="s">
-        <v>476</v>
+        <v>343</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>363</v>
+        <v>218</v>
       </c>
       <c r="B97" t="s">
-        <v>364</v>
+        <v>219</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>369</v>
+        <v>402</v>
       </c>
       <c r="B98" t="s">
-        <v>370</v>
+        <v>403</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>52</v>
+        <v>311</v>
       </c>
       <c r="B99" t="s">
-        <v>352</v>
+        <v>312</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>218</v>
+        <v>434</v>
       </c>
       <c r="B100" t="s">
-        <v>219</v>
+        <v>435</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>411</v>
+        <v>285</v>
       </c>
       <c r="B101" t="s">
-        <v>412</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>320</v>
+        <v>84</v>
       </c>
       <c r="B102" t="s">
-        <v>321</v>
+        <v>211</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>443</v>
+        <v>224</v>
       </c>
       <c r="B103" t="s">
-        <v>444</v>
+        <v>225</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>290</v>
+        <v>432</v>
       </c>
       <c r="B104" t="s">
-        <v>291</v>
+        <v>433</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>84</v>
+        <v>226</v>
       </c>
       <c r="B105" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>226</v>
+        <v>472</v>
       </c>
       <c r="B106" t="s">
-        <v>227</v>
+        <v>473</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>441</v>
+        <v>120</v>
       </c>
       <c r="B107" t="s">
-        <v>442</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>228</v>
+        <v>410</v>
       </c>
       <c r="B108" t="s">
-        <v>229</v>
+        <v>411</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>481</v>
+        <v>146</v>
       </c>
       <c r="B109" t="s">
-        <v>482</v>
+        <v>248</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>120</v>
+        <v>174</v>
       </c>
       <c r="B110" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>419</v>
+        <v>266</v>
       </c>
       <c r="B111" t="s">
-        <v>420</v>
+        <v>267</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>146</v>
+        <v>478</v>
       </c>
       <c r="B112" t="s">
-        <v>251</v>
+        <v>479</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>329</v>
       </c>
       <c r="B113" t="s">
-        <v>237</v>
+        <v>330</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>271</v>
+        <v>382</v>
       </c>
       <c r="B114" t="s">
-        <v>272</v>
+        <v>383</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="B115" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>338</v>
+        <v>438</v>
       </c>
       <c r="B116" t="s">
-        <v>339</v>
+        <v>439</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>391</v>
+        <v>412</v>
       </c>
       <c r="B117" t="s">
-        <v>392</v>
+        <v>413</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>485</v>
+        <v>315</v>
       </c>
       <c r="B118" t="s">
-        <v>486</v>
+        <v>316</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>447</v>
+        <v>333</v>
       </c>
       <c r="B119" t="s">
-        <v>448</v>
+        <v>334</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>421</v>
+        <v>350</v>
       </c>
       <c r="B120" t="s">
-        <v>422</v>
+        <v>351</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>324</v>
+        <v>436</v>
       </c>
       <c r="B121" t="s">
-        <v>325</v>
+        <v>437</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>301</v>
+        <v>388</v>
       </c>
       <c r="B122" t="s">
-        <v>302</v>
+        <v>389</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>342</v>
+        <v>422</v>
       </c>
       <c r="B123" t="s">
-        <v>343</v>
+        <v>423</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>359</v>
+        <v>392</v>
       </c>
       <c r="B124" t="s">
-        <v>360</v>
+        <v>393</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>445</v>
+        <v>456</v>
       </c>
       <c r="B125" t="s">
-        <v>446</v>
+        <v>457</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>397</v>
+        <v>235</v>
       </c>
       <c r="B126" t="s">
-        <v>398</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>431</v>
+        <v>297</v>
       </c>
       <c r="B127" t="s">
-        <v>432</v>
+        <v>298</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>401</v>
+        <v>303</v>
       </c>
       <c r="B128" t="s">
-        <v>402</v>
+        <v>304</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>465</v>
+        <v>244</v>
       </c>
       <c r="B129" t="s">
-        <v>466</v>
+        <v>245</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="B130" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>306</v>
+        <v>154</v>
       </c>
       <c r="B131" t="s">
-        <v>307</v>
+        <v>261</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>312</v>
+        <v>237</v>
       </c>
       <c r="B132" t="s">
-        <v>313</v>
+        <v>238</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>247</v>
+        <v>293</v>
       </c>
       <c r="B133" t="s">
-        <v>248</v>
+        <v>294</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>252</v>
+        <v>331</v>
       </c>
       <c r="B134" t="s">
-        <v>253</v>
+        <v>332</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>154</v>
+        <v>426</v>
       </c>
       <c r="B135" t="s">
-        <v>264</v>
+        <v>427</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="B136" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>298</v>
+        <v>256</v>
       </c>
       <c r="B137" t="s">
-        <v>299</v>
+        <v>255</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>340</v>
+        <v>452</v>
       </c>
       <c r="B138" t="s">
-        <v>341</v>
+        <v>453</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>435</v>
+        <v>408</v>
       </c>
       <c r="B139" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="B140" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>259</v>
+        <v>394</v>
       </c>
       <c r="B141" t="s">
-        <v>258</v>
+        <v>395</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>461</v>
+        <v>398</v>
       </c>
       <c r="B142" t="s">
-        <v>462</v>
+        <v>399</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>417</v>
+        <v>88</v>
       </c>
       <c r="B143" t="s">
-        <v>418</v>
+        <v>216</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>249</v>
+        <v>337</v>
       </c>
       <c r="B144" t="s">
-        <v>250</v>
+        <v>338</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>403</v>
+        <v>273</v>
       </c>
       <c r="B145" t="s">
-        <v>404</v>
+        <v>274</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B146" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>88</v>
+        <v>446</v>
       </c>
       <c r="B147" t="s">
-        <v>216</v>
+        <v>447</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>346</v>
+        <v>305</v>
       </c>
       <c r="B148" t="s">
-        <v>347</v>
+        <v>306</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>278</v>
+        <v>454</v>
       </c>
       <c r="B149" t="s">
-        <v>279</v>
+        <v>455</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>413</v>
+        <v>356</v>
       </c>
       <c r="B150" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2">
-      <c r="A151" t="s">
-        <v>455</v>
-      </c>
-      <c r="B151" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2">
-      <c r="A152" t="s">
-        <v>314</v>
-      </c>
-      <c r="B152" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2">
-      <c r="A153" t="s">
-        <v>463</v>
-      </c>
-      <c r="B153" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" t="s">
-        <v>365</v>
-      </c>
-      <c r="B154" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B154">
-    <sortCondition ref="A1:A154"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B150">
+    <sortCondition ref="A1:A150"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4399,10 +4350,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049E8705-5E6F-4E96-81BF-5F3EB9A951C5}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -4417,186 +4368,194 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="B2" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="B3" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="B4" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="B5" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="B6" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="B7" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="B8" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="B9" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="B10" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="B11" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
       <c r="B12" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="B13" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="B14" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
       <c r="B15" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="B16" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
       <c r="B17" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="B18" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="B19" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
       <c r="B20" t="s">
-        <v>540</v>
+        <v>531</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="B21" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
       <c r="B22" t="s">
-        <v>544</v>
+        <v>535</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
       <c r="B23" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="B24" t="s">
-        <v>548</v>
+        <v>539</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>541</v>
+      </c>
+      <c r="B25" t="s">
+        <v>542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>